<commit_message>
Finished Tests in Driver, fixed tree design
</commit_message>
<xml_diff>
--- a/MerkleTreeUML.xlsx
+++ b/MerkleTreeUML.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gcpet\Documents\GitHub\MerkleTree314\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/491c000d634456ab/Documents/GitHub/MerkleTree314/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C1927A-52C1-454E-9D52-B588936E2515}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{03C1927A-52C1-454E-9D52-B588936E2515}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{98A5E4E9-9D3D-4354-811A-401C674B97F3}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1520D7AD-6953-4846-AF81-F4331C007D4C}"/>
+    <workbookView xWindow="5740" yWindow="2867" windowWidth="15293" windowHeight="8473" xr2:uid="{1520D7AD-6953-4846-AF81-F4331C007D4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>Crytocurrency Transaction Merkle Tree Implementation</t>
   </si>
@@ -90,18 +81,12 @@
     <t>+ getSize() : int</t>
   </si>
   <si>
-    <t>+ getMd5() : String</t>
-  </si>
-  <si>
     <t>+ log2() : int</t>
   </si>
   <si>
     <t>+ ispowoftwo() : bool</t>
   </si>
   <si>
-    <t>- crypto() : void</t>
-  </si>
-  <si>
     <t>+ updateHash() : String</t>
   </si>
   <si>
@@ -133,6 +118,9 @@
   </si>
   <si>
     <t>- amount : double</t>
+  </si>
+  <si>
+    <t>+calcHash() : String</t>
   </si>
 </sst>
 </file>
@@ -693,157 +681,155 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D54AD8AB-501F-4FD9-B007-DEE01EEF4F95}">
   <dimension ref="E2:H37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="81" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="81" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="5" max="5" width="33.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.77734375" customWidth="1"/>
+    <col min="5" max="5" width="33.234375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.76171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="5:5" x14ac:dyDescent="0.5">
       <c r="E2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="5:5" x14ac:dyDescent="0.5">
       <c r="E4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="5:5" x14ac:dyDescent="0.5">
       <c r="E5" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="5:5" x14ac:dyDescent="0.5">
       <c r="E6" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="5:5" x14ac:dyDescent="0.5">
       <c r="E7" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="5:5" x14ac:dyDescent="0.5">
       <c r="E8" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="5:5" x14ac:dyDescent="0.5">
       <c r="E9" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="5:5" x14ac:dyDescent="0.5">
       <c r="E10" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="5:5" x14ac:dyDescent="0.5">
       <c r="E11" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="5:5" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="5:5" x14ac:dyDescent="0.5">
       <c r="E12" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="5:5" x14ac:dyDescent="0.5">
       <c r="E13" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="5:5" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="5:5" x14ac:dyDescent="0.5">
       <c r="E14" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="5:5" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="5:5" x14ac:dyDescent="0.5">
       <c r="E15" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="5:5" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="5:5" x14ac:dyDescent="0.5">
       <c r="E16" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E17" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="5:8" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="5:8" hidden="1" x14ac:dyDescent="0.5">
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="5:8" x14ac:dyDescent="0.5">
       <c r="E18" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:8" x14ac:dyDescent="0.5">
       <c r="E19" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="5:8" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="5:8" x14ac:dyDescent="0.5">
       <c r="E20" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="5:8" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="5:8" x14ac:dyDescent="0.5">
       <c r="E21" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:8" x14ac:dyDescent="0.5">
       <c r="E22" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="5:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="5:8" x14ac:dyDescent="0.5">
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="5:8" x14ac:dyDescent="0.5">
       <c r="E28" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="5:8" x14ac:dyDescent="0.5">
       <c r="E29" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H29" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="5:8" x14ac:dyDescent="0.5">
       <c r="E30" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="5:8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="5:8" x14ac:dyDescent="0.5">
       <c r="E31" s="5" t="s">
         <v>17</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="5:8" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="5:8" x14ac:dyDescent="0.5">
       <c r="E32" s="5" t="s">
         <v>16</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="5:8" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="5:8" x14ac:dyDescent="0.5">
       <c r="E33" s="5" t="s">
         <v>15</v>
       </c>
@@ -851,7 +837,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="5:8" x14ac:dyDescent="0.5">
       <c r="E34" s="5" t="s">
         <v>14</v>
       </c>
@@ -859,22 +845,22 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="5:8" x14ac:dyDescent="0.5">
       <c r="E35" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="5:8" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="5:8" x14ac:dyDescent="0.5">
       <c r="E36" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="5:8" x14ac:dyDescent="0.5">
       <c r="E37" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>